<commit_message>
add short note paper on Data Quality to references
</commit_message>
<xml_diff>
--- a/DataQuality_Models.xlsx
+++ b/DataQuality_Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ozminerals-my.sharepoint.com/personal/richard_scott_ozminerals_com/Documents/Exploration/Geoscience-Data-Quality-for-Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{34DC4501-B446-489E-96F6-9298FA39CBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0A766804-7706-41E8-B841-38A463FBC475}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{34DC4501-B446-489E-96F6-9298FA39CBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A7A9896A-878C-4EFF-9ABF-B24911E6D85B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9DEDE5E-4471-4F5A-AC8B-D4F64EE1811C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="133">
   <si>
     <t>Dataset</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Morphology</t>
   </si>
   <si>
-    <t>Incorrect Bits</t>
-  </si>
-  <si>
     <t>https://ecat.ga.gov.au/geonetwork/srv/eng/catalog.search#/metadata/89604</t>
   </si>
   <si>
@@ -289,6 +286,153 @@
   </si>
   <si>
     <t>AlOH_Group_Content</t>
+  </si>
+  <si>
+    <t>Fault lines from 1M geology</t>
+  </si>
+  <si>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>Contact lines from 1M geology</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>SEEBaseExploracorn</t>
+  </si>
+  <si>
+    <t>HydroLithology</t>
+  </si>
+  <si>
+    <t>HydroGeology</t>
+  </si>
+  <si>
+    <t>Catchments-line</t>
+  </si>
+  <si>
+    <t>Depth to Basement</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>lithology2-lithology</t>
+  </si>
+  <si>
+    <t>Lithology rolled up to 55 classes</t>
+  </si>
+  <si>
+    <t>2019_A4_CBA_ONSHORE</t>
+  </si>
+  <si>
+    <t>2019_A4_CBA_ONSHORE_1VDGRAV</t>
+  </si>
+  <si>
+    <t>2019_A7_DGIR_ONSHORE</t>
+  </si>
+  <si>
+    <t>2019_A7_DGIR_ONSHORE_1VDGRAV</t>
+  </si>
+  <si>
+    <t>Total Magnetic Intensity grid of Australia 2019 80m.tif</t>
+  </si>
+  <si>
+    <t>radmap_v4_2019_filtered_ppmu</t>
+  </si>
+  <si>
+    <t>magmap_v7_2019_1VD</t>
+  </si>
+  <si>
+    <t>magmap_v7_2019_RTP</t>
+  </si>
+  <si>
+    <t>radmap_v4_2019_filtered_dose</t>
+  </si>
+  <si>
+    <t>Total Magnetic Intensity grid of Australia 2019 40m.tif</t>
+  </si>
+  <si>
+    <t>radmap_v4_2019_filtered_ppmth</t>
+  </si>
+  <si>
+    <t>radmap_v4_2019_filtered_pctk</t>
+  </si>
+  <si>
+    <t>Y14</t>
+  </si>
+  <si>
+    <t>twi_3s</t>
+  </si>
+  <si>
+    <t>national_Wii_RF</t>
+  </si>
+  <si>
+    <t>FR12</t>
+  </si>
+  <si>
+    <t>AusREM</t>
+  </si>
+  <si>
+    <t>Seismic</t>
+  </si>
+  <si>
+    <t>DER_000_999_EV_N_P_AU_NAT_C_20150601</t>
+  </si>
+  <si>
+    <t>Depth of Regolith 2</t>
+  </si>
+  <si>
+    <t>https://data.csiro.au/collections/collection/CIcsiro:5588/SQtopographical%20wetness%20index/RP1/RS25/RORELEVANCE/STsearch-by-keyword/RI1/RT3/</t>
+  </si>
+  <si>
+    <t>Topographic Wetness Index derived from 1" SRTM DEM-H -3" derived version</t>
+  </si>
+  <si>
+    <t>Wetness Index</t>
+  </si>
+  <si>
+    <t>Weathering Intensity</t>
+  </si>
+  <si>
+    <t>Hydrology</t>
+  </si>
+  <si>
+    <t>https://ecat.ga.gov.au/geonetwork/srv/eng/catalog.search#/metadata/131978</t>
+  </si>
+  <si>
+    <t>https://ecat.ga.gov.au/geonetwork/srv/eng/catalog.search#/metadata/131974</t>
+  </si>
+  <si>
+    <t>https://ecat.ga.gov.au/geonetwork/srv/eng/catalog.search#/metadata/131988</t>
+  </si>
+  <si>
+    <t>http://http://rses.anu.edu.au/seismology/AuSREM/AusMoho/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work in progress - </t>
+  </si>
+  <si>
+    <t>https://osf.io/twksd/</t>
+  </si>
+  <si>
+    <t>https://researchdata.edu.au/weathering-intensity-model-australia/1361069</t>
+  </si>
+  <si>
+    <t>https://data.csiro.au/collections/collection/CI29936</t>
+  </si>
+  <si>
+    <t>https://ecat.ga.gov.au/geonetwork/srv/eng/catalog.search#/metadata/32368</t>
+  </si>
+  <si>
+    <t>https://www.geognostics.com/seebase-depth-to-basement</t>
+  </si>
+  <si>
+    <t>AusMoho</t>
   </si>
 </sst>
 </file>
@@ -373,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -389,6 +533,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -704,11 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63D4C59-F36B-48A1-AE9A-D5AD99EC9BB5}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -722,6 +869,8 @@
     <col min="8" max="8" width="11.109375" customWidth="1"/>
     <col min="9" max="9" width="67.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="73.5546875" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -741,13 +890,13 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -760,6 +909,9 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -797,7 +949,7 @@
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
         <v>13</v>
@@ -841,7 +993,7 @@
         <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
         <v>13</v>
@@ -862,15 +1014,15 @@
         <v>1</v>
       </c>
       <c r="D4" s="8">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E5" si="2">1/D4</f>
-        <v>1.1111111111111112E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11.25</v>
       </c>
       <c r="G4">
         <v>2015</v>
@@ -879,19 +1031,19 @@
         <v>4</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" t="s">
         <v>72</v>
-      </c>
-      <c r="K4" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" t="s">
-        <v>74</v>
-      </c>
-      <c r="M4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -906,15 +1058,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="8">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="2"/>
-        <v>1.1111111111111112E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11.25</v>
       </c>
       <c r="G5">
         <v>2015</v>
@@ -929,13 +1081,13 @@
         <v>60</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1500,19 +1652,19 @@
         <v>4</v>
       </c>
       <c r="I19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L19" t="s">
         <v>49</v>
       </c>
       <c r="M19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1547,13 +1699,13 @@
         <v>35</v>
       </c>
       <c r="K20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L20" t="s">
         <v>49</v>
       </c>
       <c r="M20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1588,13 +1740,13 @@
         <v>35</v>
       </c>
       <c r="K21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L21" t="s">
         <v>49</v>
       </c>
       <c r="M21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1629,13 +1781,13 @@
         <v>35</v>
       </c>
       <c r="K22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L22" t="s">
         <v>49</v>
       </c>
       <c r="M22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1678,7 +1830,7 @@
         <v>47</v>
       </c>
       <c r="M23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1870,7 +2022,7 @@
         <v>48</v>
       </c>
       <c r="L28" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1887,6 +2039,9 @@
       <c r="I29" t="s">
         <v>55</v>
       </c>
+      <c r="J29" t="s">
+        <v>84</v>
+      </c>
       <c r="K29" t="s">
         <v>48</v>
       </c>
@@ -1896,7 +2051,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -1919,34 +2074,34 @@
         <v>2019</v>
       </c>
       <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" t="s">
         <v>77</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="K30" t="s">
         <v>79</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>80</v>
       </c>
-      <c r="L30" t="s">
-        <v>81</v>
-      </c>
       <c r="M30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" s="7">
-        <f>48.27/48.27</f>
-        <v>1</v>
+        <f>35.52/35.76*C32</f>
+        <v>0.98491216201097476</v>
       </c>
       <c r="D31">
         <v>90</v>
@@ -1956,8 +2111,8 @@
         <v>1.1111111111111112E-2</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" ref="F31:F32" si="8">ROUND(B31*C31*E31*100*3,2)</f>
-        <v>6.67</v>
+        <f t="shared" ref="F31:F33" si="8">ROUND(B31*C31*E31*100*3,2)</f>
+        <v>6.57</v>
       </c>
       <c r="G31">
         <v>2012</v>
@@ -1977,14 +2132,14 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" ref="C32" si="9">48.27/48.27</f>
-        <v>1</v>
+        <f>50.56/50.99</f>
+        <v>0.99156697391645421</v>
       </c>
       <c r="D32">
         <v>90</v>
@@ -1995,7 +2150,7 @@
       </c>
       <c r="F32" s="4">
         <f t="shared" si="8"/>
-        <v>6.67</v>
+        <v>6.61</v>
       </c>
       <c r="G32">
         <v>2012</v>
@@ -2013,8 +2168,964 @@
         <v>30</v>
       </c>
     </row>
+    <row r="33" spans="1:13">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D33">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" ref="E33" si="9">1/D33</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="8"/>
+        <v>0.2</v>
+      </c>
+      <c r="G33">
+        <v>2012</v>
+      </c>
+      <c r="H33" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" t="s">
+        <v>62</v>
+      </c>
+      <c r="K33" t="s">
+        <v>48</v>
+      </c>
+      <c r="L33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D34">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" ref="E34:E35" si="10">1/D34</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" ref="F34:F35" si="11">ROUND(B34*C34*E34*100*3,2)</f>
+        <v>0.2</v>
+      </c>
+      <c r="G34">
+        <v>2012</v>
+      </c>
+      <c r="H34" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K34" t="s">
+        <v>48</v>
+      </c>
+      <c r="L34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>12000</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="10"/>
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="11"/>
+        <v>0.05</v>
+      </c>
+      <c r="G35">
+        <v>2020</v>
+      </c>
+      <c r="H35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>131</v>
+      </c>
+      <c r="K35" t="s">
+        <v>48</v>
+      </c>
+      <c r="L35" t="s">
+        <v>93</v>
+      </c>
+      <c r="M35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>5000</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" ref="E36:E38" si="12">1/D36</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F36" s="4">
+        <f t="shared" ref="F36:F38" si="13">ROUND(B36*C36*E36*100*3,2)</f>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1987</v>
+      </c>
+      <c r="H36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K36" t="s">
+        <v>48</v>
+      </c>
+      <c r="L36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="12"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F37" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>1987</v>
+      </c>
+      <c r="H37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K37" t="s">
+        <v>48</v>
+      </c>
+      <c r="L37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="7">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>5000</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="12"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F38" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>1987</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K38" t="s">
+        <v>48</v>
+      </c>
+      <c r="L38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1000</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" ref="E39:E54" si="14">1/D39</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F39" s="4">
+        <f t="shared" ref="F39:F54" si="15">ROUND(B39*C39*E39*100*3,2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="G39">
+        <v>2012</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" t="s">
+        <v>62</v>
+      </c>
+      <c r="J39" t="s">
+        <v>96</v>
+      </c>
+      <c r="K39" t="s">
+        <v>48</v>
+      </c>
+      <c r="L39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>400</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="14"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F40" s="4">
+        <f t="shared" si="15"/>
+        <v>2.25</v>
+      </c>
+      <c r="G40">
+        <v>2019</v>
+      </c>
+      <c r="H40" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" t="s">
+        <v>79</v>
+      </c>
+      <c r="L40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>400</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="14"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F41" s="4">
+        <f t="shared" si="15"/>
+        <v>2.25</v>
+      </c>
+      <c r="G41">
+        <v>2019</v>
+      </c>
+      <c r="H41" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" t="s">
+        <v>79</v>
+      </c>
+      <c r="L41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>400</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" si="14"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F42" s="4">
+        <f t="shared" si="15"/>
+        <v>2.25</v>
+      </c>
+      <c r="G42">
+        <v>2019</v>
+      </c>
+      <c r="H42" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" t="s">
+        <v>79</v>
+      </c>
+      <c r="L42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>400</v>
+      </c>
+      <c r="E43" s="4">
+        <f t="shared" si="14"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F43" s="4">
+        <f t="shared" si="15"/>
+        <v>2.25</v>
+      </c>
+      <c r="G43">
+        <v>2019</v>
+      </c>
+      <c r="H43" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" t="s">
+        <v>79</v>
+      </c>
+      <c r="L43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>80</v>
+      </c>
+      <c r="E44" s="4">
+        <f t="shared" si="14"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="F44" s="4">
+        <f t="shared" si="15"/>
+        <v>11.25</v>
+      </c>
+      <c r="G44">
+        <v>2019</v>
+      </c>
+      <c r="H44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" t="s">
+        <v>79</v>
+      </c>
+      <c r="L44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" s="7">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>40</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="14"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F45" s="4">
+        <f t="shared" si="15"/>
+        <v>22.5</v>
+      </c>
+      <c r="G45">
+        <v>2019</v>
+      </c>
+      <c r="H45" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" t="s">
+        <v>79</v>
+      </c>
+      <c r="L45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>80</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" si="14"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="F46" s="4">
+        <f t="shared" si="15"/>
+        <v>11.25</v>
+      </c>
+      <c r="G46">
+        <v>2019</v>
+      </c>
+      <c r="H46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K46" t="s">
+        <v>79</v>
+      </c>
+      <c r="L46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" s="7">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>80</v>
+      </c>
+      <c r="E47" s="4">
+        <f t="shared" si="14"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="F47" s="4">
+        <f t="shared" si="15"/>
+        <v>11.25</v>
+      </c>
+      <c r="G47">
+        <v>2019</v>
+      </c>
+      <c r="H47" t="s">
+        <v>4</v>
+      </c>
+      <c r="K47" t="s">
+        <v>79</v>
+      </c>
+      <c r="L47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" s="7">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>110</v>
+      </c>
+      <c r="E48" s="4">
+        <f t="shared" si="14"/>
+        <v>9.0909090909090905E-3</v>
+      </c>
+      <c r="F48" s="4">
+        <f t="shared" si="15"/>
+        <v>8.18</v>
+      </c>
+      <c r="G48">
+        <v>2019</v>
+      </c>
+      <c r="H48" t="s">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s">
+        <v>79</v>
+      </c>
+      <c r="L48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" s="7">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>110</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" si="14"/>
+        <v>9.0909090909090905E-3</v>
+      </c>
+      <c r="F49" s="4">
+        <f t="shared" si="15"/>
+        <v>8.18</v>
+      </c>
+      <c r="G49">
+        <v>2019</v>
+      </c>
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+      <c r="I49" t="s">
+        <v>123</v>
+      </c>
+      <c r="K49" t="s">
+        <v>79</v>
+      </c>
+      <c r="L49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>110</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="14"/>
+        <v>9.0909090909090905E-3</v>
+      </c>
+      <c r="F50" s="4">
+        <f t="shared" si="15"/>
+        <v>8.18</v>
+      </c>
+      <c r="G50">
+        <v>2019</v>
+      </c>
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K50" t="s">
+        <v>79</v>
+      </c>
+      <c r="L50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" s="7">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>110</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" si="14"/>
+        <v>9.0909090909090905E-3</v>
+      </c>
+      <c r="F51" s="4">
+        <f t="shared" si="15"/>
+        <v>8.18</v>
+      </c>
+      <c r="G51">
+        <v>2019</v>
+      </c>
+      <c r="H51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51" t="s">
+        <v>122</v>
+      </c>
+      <c r="K51" t="s">
+        <v>79</v>
+      </c>
+      <c r="L51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" s="7">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>10000</v>
+      </c>
+      <c r="E52" s="4">
+        <f t="shared" si="14"/>
+        <v>1E-4</v>
+      </c>
+      <c r="F52" s="4">
+        <f t="shared" si="15"/>
+        <v>0.06</v>
+      </c>
+      <c r="G52">
+        <v>2020</v>
+      </c>
+      <c r="H52" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K52" t="s">
+        <v>79</v>
+      </c>
+      <c r="L52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>10000</v>
+      </c>
+      <c r="E53" s="4">
+        <f t="shared" si="14"/>
+        <v>1E-4</v>
+      </c>
+      <c r="F53" s="4">
+        <f t="shared" si="15"/>
+        <v>0.06</v>
+      </c>
+      <c r="G53">
+        <v>2020</v>
+      </c>
+      <c r="H53" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K53" t="s">
+        <v>79</v>
+      </c>
+      <c r="L53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>10000</v>
+      </c>
+      <c r="E54" s="4">
+        <f t="shared" si="14"/>
+        <v>1E-4</v>
+      </c>
+      <c r="F54" s="4">
+        <f t="shared" si="15"/>
+        <v>0.06</v>
+      </c>
+      <c r="G54">
+        <v>2020</v>
+      </c>
+      <c r="H54" t="s">
+        <v>4</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K54" t="s">
+        <v>79</v>
+      </c>
+      <c r="L54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1000</v>
+      </c>
+      <c r="E55" s="4">
+        <f t="shared" ref="E55:E56" si="16">1/D55</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F55" s="4">
+        <f t="shared" ref="F55:F56" si="17">ROUND(B55*C55*E55*100*3,2)</f>
+        <v>0.6</v>
+      </c>
+      <c r="G55">
+        <v>2016</v>
+      </c>
+      <c r="H55" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55" t="s">
+        <v>117</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K55" t="s">
+        <v>45</v>
+      </c>
+      <c r="L55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" s="7">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1000</v>
+      </c>
+      <c r="E56" s="4">
+        <f t="shared" si="16"/>
+        <v>1E-3</v>
+      </c>
+      <c r="F56" s="4">
+        <f t="shared" si="17"/>
+        <v>0.6</v>
+      </c>
+      <c r="G56">
+        <v>2015</v>
+      </c>
+      <c r="H56" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56" t="s">
+        <v>128</v>
+      </c>
+      <c r="K56" t="s">
+        <v>45</v>
+      </c>
+      <c r="L56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>90</v>
+      </c>
+      <c r="E57" s="4">
+        <f t="shared" ref="E57:E58" si="18">1/D57</f>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="F57" s="4">
+        <f t="shared" ref="F57:F58" si="19">ROUND(B57*C57*E57*100*3,2)</f>
+        <v>6.67</v>
+      </c>
+      <c r="G57">
+        <v>2018</v>
+      </c>
+      <c r="H57" t="s">
+        <v>4</v>
+      </c>
+      <c r="I57" t="s">
+        <v>129</v>
+      </c>
+      <c r="J57" t="s">
+        <v>116</v>
+      </c>
+      <c r="K57" t="s">
+        <v>48</v>
+      </c>
+      <c r="L57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" s="7">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>5000</v>
+      </c>
+      <c r="E58" s="4">
+        <f t="shared" si="18"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="F58" s="4">
+        <f t="shared" si="19"/>
+        <v>0.12</v>
+      </c>
+      <c r="G58">
+        <v>2020</v>
+      </c>
+      <c r="H58" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K58" t="s">
+        <v>79</v>
+      </c>
+      <c r="L58" t="s">
+        <v>114</v>
+      </c>
+      <c r="M58" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I50" r:id="rId1" location="/metadata/131988" xr:uid="{B220D465-DA1C-4A0D-A692-C842A95FE5F2}"/>
+    <hyperlink ref="I58" r:id="rId2" xr:uid="{2E3D4E5B-A2BF-4891-945A-0ACA39A140AA}"/>
+    <hyperlink ref="I52" r:id="rId3" display="https://protect-au.mimecast.com/s/0Yd9CYWL4jILNYEAi0-ij7?domain=osf.io/" xr:uid="{9DC39983-D2E9-421E-B4B3-A0D0995BB0BF}"/>
+    <hyperlink ref="I53" r:id="rId4" display="https://protect-au.mimecast.com/s/0Yd9CYWL4jILNYEAi0-ij7?domain=osf.io/" xr:uid="{800D1A09-A20D-48CE-A3BB-2013201C2F45}"/>
+    <hyperlink ref="I54" r:id="rId5" display="https://protect-au.mimecast.com/s/0Yd9CYWL4jILNYEAi0-ij7?domain=osf.io/" xr:uid="{7DDF99EC-A458-4184-A9B4-3BE563863137}"/>
+    <hyperlink ref="I38" r:id="rId6" location="/metadata/32368" xr:uid="{0ABA7C62-409C-426D-A626-2A8A6ED63EBD}"/>
+    <hyperlink ref="I37" r:id="rId7" location="/metadata/32368" xr:uid="{2A097C8C-8CE4-4A56-A774-08985F743228}"/>
+    <hyperlink ref="I36" r:id="rId8" location="/metadata/32368" xr:uid="{3F4399DD-3529-4F4D-B07C-8B8924594C84}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2019 rad area update
</commit_message>
<xml_diff>
--- a/DataQuality_Models.xlsx
+++ b/DataQuality_Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ozminerals-my.sharepoint.com/personal/richard_scott_ozminerals_com/Documents/Exploration/Geoscience-Data-Quality-for-Machine-Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="8_{34DC4501-B446-489E-96F6-9298FA39CBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{73B1DE10-58CD-4712-B49B-E50F9FD8F345}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{34DC4501-B446-489E-96F6-9298FA39CBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4FFB34DC-385C-4BB3-8CB3-3A4C9406A8B5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9DEDE5E-4471-4F5A-AC8B-D4F64EE1811C}"/>
   </bookViews>
@@ -898,9 +898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63D4C59-F36B-48A1-AE9A-D5AD99EC9BB5}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2778,7 +2778,8 @@
         <v>3</v>
       </c>
       <c r="C48" s="7">
-        <v>1</v>
+        <f t="shared" ref="C48:C51" si="16">47.23/48.27</f>
+        <v>0.97845452662108956</v>
       </c>
       <c r="D48">
         <v>110</v>
@@ -2789,7 +2790,7 @@
       </c>
       <c r="F48" s="4">
         <f t="shared" si="15"/>
-        <v>8.18</v>
+        <v>8.01</v>
       </c>
       <c r="G48">
         <v>2019</v>
@@ -2818,7 +2819,8 @@
         <v>3</v>
       </c>
       <c r="C49" s="7">
-        <v>1</v>
+        <f t="shared" si="16"/>
+        <v>0.97845452662108956</v>
       </c>
       <c r="D49">
         <v>110</v>
@@ -2829,7 +2831,7 @@
       </c>
       <c r="F49" s="4">
         <f t="shared" si="15"/>
-        <v>8.18</v>
+        <v>8.01</v>
       </c>
       <c r="G49">
         <v>2019</v>
@@ -2858,7 +2860,8 @@
         <v>3</v>
       </c>
       <c r="C50" s="7">
-        <v>1</v>
+        <f t="shared" si="16"/>
+        <v>0.97845452662108956</v>
       </c>
       <c r="D50">
         <v>110</v>
@@ -2869,7 +2872,7 @@
       </c>
       <c r="F50" s="4">
         <f t="shared" si="15"/>
-        <v>8.18</v>
+        <v>8.01</v>
       </c>
       <c r="G50">
         <v>2019</v>
@@ -2898,7 +2901,8 @@
         <v>3</v>
       </c>
       <c r="C51" s="7">
-        <v>1</v>
+        <f t="shared" si="16"/>
+        <v>0.97845452662108956</v>
       </c>
       <c r="D51">
         <v>110</v>
@@ -2909,7 +2913,7 @@
       </c>
       <c r="F51" s="4">
         <f t="shared" si="15"/>
-        <v>8.18</v>
+        <v>8.01</v>
       </c>
       <c r="G51">
         <v>2019</v>
@@ -3055,11 +3059,11 @@
         <v>1000</v>
       </c>
       <c r="E55" s="4">
-        <f t="shared" ref="E55:E56" si="16">1/D55</f>
+        <f t="shared" ref="E55:E56" si="17">1/D55</f>
         <v>1E-3</v>
       </c>
       <c r="F55" s="4">
-        <f t="shared" ref="F55:F56" si="17">ROUND(B55*C55*E55*100*3,2)</f>
+        <f t="shared" ref="F55:F56" si="18">ROUND(B55*C55*E55*100*3,2)</f>
         <v>0.6</v>
       </c>
       <c r="G55">
@@ -3095,11 +3099,11 @@
         <v>1000</v>
       </c>
       <c r="E56" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
       <c r="F56" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.6</v>
       </c>
       <c r="G56">
@@ -3135,11 +3139,11 @@
         <v>90</v>
       </c>
       <c r="E57" s="4">
-        <f t="shared" ref="E57:E58" si="18">1/D57</f>
+        <f t="shared" ref="E57:E58" si="19">1/D57</f>
         <v>1.1111111111111112E-2</v>
       </c>
       <c r="F57" s="4">
-        <f t="shared" ref="F57:F58" si="19">ROUND(B57*C57*E57*100*3,2)</f>
+        <f t="shared" ref="F57:F58" si="20">ROUND(B57*C57*E57*100*3,2)</f>
         <v>6.67</v>
       </c>
       <c r="G57">
@@ -3175,11 +3179,11 @@
         <v>5000</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
       <c r="G58">

</xml_diff>